<commit_message>
Added Report and Readme
</commit_message>
<xml_diff>
--- a/results/first/table_and_plots.xlsx
+++ b/results/first/table_and_plots.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="6852" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="6852" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="max5min" sheetId="1" r:id="rId1"/>
     <sheet name="max10min" sheetId="2" r:id="rId2"/>
     <sheet name="max20min" sheetId="3" r:id="rId3"/>
+    <sheet name="Gráfico1" sheetId="5" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="brkgaMax5min" localSheetId="0">max5min!#REF!</definedName>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="57">
   <si>
     <t>dat_file</t>
   </si>
@@ -218,6 +220,15 @@
   <si>
     <t>cost_brkga</t>
   </si>
+  <si>
+    <t>max 5 min</t>
+  </si>
+  <si>
+    <t>max 10 min</t>
+  </si>
+  <si>
+    <t>max 20 min</t>
+  </si>
 </sst>
 </file>
 
@@ -252,8 +263,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,11 +862,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="386261816"/>
-        <c:axId val="386259856"/>
+        <c:axId val="256781720"/>
+        <c:axId val="256789168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="386261816"/>
+        <c:axId val="256781720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,7 +908,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386259856"/>
+        <c:crossAx val="256789168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -902,7 +916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="386259856"/>
+        <c:axId val="256789168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -953,7 +967,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386261816"/>
+        <c:crossAx val="256781720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1312,11 +1326,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="474708120"/>
-        <c:axId val="474707336"/>
+        <c:axId val="470033968"/>
+        <c:axId val="470037888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="474708120"/>
+        <c:axId val="470033968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1358,7 +1372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474707336"/>
+        <c:crossAx val="470037888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1366,7 +1380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="474707336"/>
+        <c:axId val="470037888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +1431,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474708120"/>
+        <c:crossAx val="470033968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1765,11 +1779,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="479198472"/>
-        <c:axId val="479198864"/>
+        <c:axId val="470030048"/>
+        <c:axId val="470033184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="479198472"/>
+        <c:axId val="470030048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,7 +1825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479198864"/>
+        <c:crossAx val="470033184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1819,7 +1833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479198864"/>
+        <c:axId val="470033184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1870,7 +1884,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479198472"/>
+        <c:crossAx val="470030048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2206,11 +2220,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="34054776"/>
-        <c:axId val="34055168"/>
+        <c:axId val="470031224"/>
+        <c:axId val="470037496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="34054776"/>
+        <c:axId val="470031224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2252,7 +2266,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34055168"/>
+        <c:crossAx val="470037496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2260,7 +2274,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34055168"/>
+        <c:axId val="470037496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2311,7 +2325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34054776"/>
+        <c:crossAx val="470031224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3008,11 +3022,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="480793480"/>
-        <c:axId val="480799360"/>
+        <c:axId val="470028480"/>
+        <c:axId val="470031616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="480793480"/>
+        <c:axId val="470028480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3054,7 +3068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480799360"/>
+        <c:crossAx val="470031616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3062,7 +3076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="480799360"/>
+        <c:axId val="470031616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3113,7 +3127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480793480"/>
+        <c:crossAx val="470028480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3473,11 +3487,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="385943368"/>
-        <c:axId val="385942584"/>
+        <c:axId val="470030832"/>
+        <c:axId val="470029264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="385943368"/>
+        <c:axId val="470030832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3519,7 +3533,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385942584"/>
+        <c:crossAx val="470029264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3527,7 +3541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="385942584"/>
+        <c:axId val="470029264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3578,7 +3592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385943368"/>
+        <c:crossAx val="470030832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3938,11 +3952,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="479212584"/>
-        <c:axId val="479211408"/>
+        <c:axId val="470032008"/>
+        <c:axId val="470026912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="479212584"/>
+        <c:axId val="470032008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3984,7 +3998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479211408"/>
+        <c:crossAx val="470026912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3992,7 +4006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479211408"/>
+        <c:axId val="470026912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4043,7 +4057,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479212584"/>
+        <c:crossAx val="470032008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4370,11 +4384,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="476191456"/>
-        <c:axId val="473292464"/>
+        <c:axId val="470032792"/>
+        <c:axId val="470036712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="476191456"/>
+        <c:axId val="470032792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4416,7 +4430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473292464"/>
+        <c:crossAx val="470036712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4424,7 +4438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="473292464"/>
+        <c:axId val="470036712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4475,7 +4489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476191456"/>
+        <c:crossAx val="470032792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4829,11 +4843,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="477372128"/>
-        <c:axId val="477367032"/>
+        <c:axId val="470033576"/>
+        <c:axId val="470034360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="477372128"/>
+        <c:axId val="470033576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4875,7 +4889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477367032"/>
+        <c:crossAx val="470034360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4883,7 +4897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="477367032"/>
+        <c:axId val="470034360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4934,7 +4948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477372128"/>
+        <c:crossAx val="470033576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5270,11 +5284,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="337590848"/>
-        <c:axId val="337592024"/>
+        <c:axId val="470028088"/>
+        <c:axId val="470034752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="337590848"/>
+        <c:axId val="470028088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5316,7 +5330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337592024"/>
+        <c:crossAx val="470034752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5324,7 +5338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="337592024"/>
+        <c:axId val="470034752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5375,7 +5389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337590848"/>
+        <c:crossAx val="470028088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5453,6 +5467,778 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Comparison of performance vs maxTime</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max 5 min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Hoja1!$B$21:$S$22</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>cost_opl</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>cost_grasp</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>cost_brkga</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$23:$S$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2286</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2374</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2460</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1762</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1906</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1968</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1811</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1858</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1968</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2138</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max 10 min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Hoja1!$B$21:$S$22</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>cost_opl</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>cost_grasp</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>cost_brkga</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$24:$S$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2286</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2374</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2460</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1758</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1809</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1907</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1968</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2052</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1784</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1839</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1947</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max 20 min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Hoja1!$B$21:$S$22</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>feasible1_31.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>feasible1_32.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>feasible1_34.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>feasible1_35.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>feasible1_36.dat</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>feasible1_37.dat</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>cost_opl</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>cost_grasp</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>cost_brkga</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$25:$S$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2286</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2374</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2460</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1761</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1808</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1906</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1968</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2059</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1771</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1819</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1923</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2076</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="474464536"/>
+        <c:axId val="479242912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="474464536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479242912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="479242912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474464536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
 </c:chartSpace>
 </file>
 
@@ -5735,11 +6521,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="385942976"/>
-        <c:axId val="385941408"/>
+        <c:axId val="256790344"/>
+        <c:axId val="256780544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="385942976"/>
+        <c:axId val="256790344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5781,7 +6567,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385941408"/>
+        <c:crossAx val="256780544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5789,7 +6575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="385941408"/>
+        <c:axId val="256780544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5840,7 +6626,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385942976"/>
+        <c:crossAx val="256790344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6200,11 +6986,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="482460248"/>
-        <c:axId val="482466520"/>
+        <c:axId val="256782504"/>
+        <c:axId val="256786424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="482460248"/>
+        <c:axId val="256782504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6246,7 +7032,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482466520"/>
+        <c:crossAx val="256786424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6254,7 +7040,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482466520"/>
+        <c:axId val="256786424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6305,7 +7091,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482460248"/>
+        <c:crossAx val="256782504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6659,11 +7445,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="474907384"/>
-        <c:axId val="474908168"/>
+        <c:axId val="256780152"/>
+        <c:axId val="256779368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="474907384"/>
+        <c:axId val="256780152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6705,7 +7491,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474908168"/>
+        <c:crossAx val="256779368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6713,7 +7499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="474908168"/>
+        <c:axId val="256779368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6764,7 +7550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474907384"/>
+        <c:crossAx val="256780152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7112,11 +7898,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="476194984"/>
-        <c:axId val="476193808"/>
+        <c:axId val="256792304"/>
+        <c:axId val="256793872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="476194984"/>
+        <c:axId val="256792304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7158,7 +7944,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476193808"/>
+        <c:crossAx val="256793872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7166,7 +7952,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="476193808"/>
+        <c:axId val="256793872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7217,7 +8003,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476194984"/>
+        <c:crossAx val="256792304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7523,11 +8309,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="476199088"/>
-        <c:axId val="476196344"/>
+        <c:axId val="256785248"/>
+        <c:axId val="256780936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="476199088"/>
+        <c:axId val="256785248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7569,7 +8355,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476196344"/>
+        <c:crossAx val="256780936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7577,7 +8363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="476196344"/>
+        <c:axId val="256780936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7628,7 +8414,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476199088"/>
+        <c:crossAx val="256785248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8319,11 +9105,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="472588048"/>
-        <c:axId val="472589224"/>
+        <c:axId val="256795048"/>
+        <c:axId val="256792696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472588048"/>
+        <c:axId val="256795048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8365,7 +9151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472589224"/>
+        <c:crossAx val="256792696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8373,7 +9159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472589224"/>
+        <c:axId val="256792696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8424,7 +9210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472588048"/>
+        <c:crossAx val="256795048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8784,11 +9570,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="479206704"/>
-        <c:axId val="479203960"/>
+        <c:axId val="256791912"/>
+        <c:axId val="256793480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="479206704"/>
+        <c:axId val="256791912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8830,7 +9616,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479203960"/>
+        <c:crossAx val="256793480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8838,7 +9624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479203960"/>
+        <c:axId val="256793480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8889,7 +9675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479206704"/>
+        <c:crossAx val="256791912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9249,11 +10035,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="34052816"/>
-        <c:axId val="34053208"/>
+        <c:axId val="470038280"/>
+        <c:axId val="470027304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="34052816"/>
+        <c:axId val="470038280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9295,7 +10081,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34053208"/>
+        <c:crossAx val="470027304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9303,7 +10089,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34053208"/>
+        <c:axId val="470027304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9354,7 +10140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34052816"/>
+        <c:crossAx val="470038280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9835,6 +10621,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -15211,7 +16037,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15714,7 +16540,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16217,7 +17043,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16720,7 +17546,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -17223,7 +18049,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -17726,8 +18552,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -17835,11 +18661,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -17850,11 +18671,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -17886,9 +18702,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -18242,8 +19055,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -18351,6 +19164,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -18361,6 +19179,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -18392,6 +19215,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -18745,7 +19571,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19246,6 +20072,521 @@
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19803,6 +21144,33 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9283290" cy="6063226"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="oplMax5min" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -20076,8 +21444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20741,8 +22109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21444,8 +22812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22145,4 +23513,766 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>2096</v>
+      </c>
+      <c r="C3">
+        <v>1762</v>
+      </c>
+      <c r="D3">
+        <v>1811</v>
+      </c>
+      <c r="E3">
+        <v>2096</v>
+      </c>
+      <c r="F3">
+        <v>1758</v>
+      </c>
+      <c r="G3">
+        <v>1784</v>
+      </c>
+      <c r="H3">
+        <v>2096</v>
+      </c>
+      <c r="I3">
+        <v>1761</v>
+      </c>
+      <c r="J3">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>2146</v>
+      </c>
+      <c r="C4">
+        <v>1810</v>
+      </c>
+      <c r="D4">
+        <v>1858</v>
+      </c>
+      <c r="E4">
+        <v>2146</v>
+      </c>
+      <c r="F4">
+        <v>1809</v>
+      </c>
+      <c r="G4">
+        <v>1839</v>
+      </c>
+      <c r="H4">
+        <v>2146</v>
+      </c>
+      <c r="I4">
+        <v>1808</v>
+      </c>
+      <c r="J4">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>2263</v>
+      </c>
+      <c r="C5">
+        <v>1906</v>
+      </c>
+      <c r="D5">
+        <v>1968</v>
+      </c>
+      <c r="E5">
+        <v>2263</v>
+      </c>
+      <c r="F5">
+        <v>1907</v>
+      </c>
+      <c r="G5">
+        <v>1947</v>
+      </c>
+      <c r="H5">
+        <v>2263</v>
+      </c>
+      <c r="I5">
+        <v>1906</v>
+      </c>
+      <c r="J5">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>2286</v>
+      </c>
+      <c r="C6">
+        <v>1968</v>
+      </c>
+      <c r="D6">
+        <v>2025</v>
+      </c>
+      <c r="E6">
+        <v>2286</v>
+      </c>
+      <c r="F6">
+        <v>1968</v>
+      </c>
+      <c r="G6">
+        <v>1997</v>
+      </c>
+      <c r="H6">
+        <v>2286</v>
+      </c>
+      <c r="I6">
+        <v>1968</v>
+      </c>
+      <c r="J6">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7">
+        <v>2374</v>
+      </c>
+      <c r="C7">
+        <v>2012</v>
+      </c>
+      <c r="D7">
+        <v>2072</v>
+      </c>
+      <c r="E7">
+        <v>2374</v>
+      </c>
+      <c r="F7">
+        <v>2010</v>
+      </c>
+      <c r="G7">
+        <v>2045</v>
+      </c>
+      <c r="H7">
+        <v>2374</v>
+      </c>
+      <c r="I7">
+        <v>2010</v>
+      </c>
+      <c r="J7">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>2460</v>
+      </c>
+      <c r="C8">
+        <v>2058</v>
+      </c>
+      <c r="D8">
+        <v>2138</v>
+      </c>
+      <c r="E8">
+        <v>2460</v>
+      </c>
+      <c r="F8">
+        <v>2052</v>
+      </c>
+      <c r="G8">
+        <v>2097</v>
+      </c>
+      <c r="H8">
+        <v>2460</v>
+      </c>
+      <c r="I8">
+        <v>2059</v>
+      </c>
+      <c r="J8">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>2096</v>
+      </c>
+      <c r="C13">
+        <v>2096</v>
+      </c>
+      <c r="D13">
+        <v>2096</v>
+      </c>
+      <c r="E13">
+        <v>1762</v>
+      </c>
+      <c r="F13">
+        <v>1758</v>
+      </c>
+      <c r="G13">
+        <v>1761</v>
+      </c>
+      <c r="H13">
+        <v>1811</v>
+      </c>
+      <c r="I13">
+        <v>1784</v>
+      </c>
+      <c r="J13">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>2146</v>
+      </c>
+      <c r="C14">
+        <v>2146</v>
+      </c>
+      <c r="D14">
+        <v>2146</v>
+      </c>
+      <c r="E14">
+        <v>1810</v>
+      </c>
+      <c r="F14">
+        <v>1809</v>
+      </c>
+      <c r="G14">
+        <v>1808</v>
+      </c>
+      <c r="H14">
+        <v>1858</v>
+      </c>
+      <c r="I14">
+        <v>1839</v>
+      </c>
+      <c r="J14">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15">
+        <v>2263</v>
+      </c>
+      <c r="C15">
+        <v>2263</v>
+      </c>
+      <c r="D15">
+        <v>2263</v>
+      </c>
+      <c r="E15">
+        <v>1906</v>
+      </c>
+      <c r="F15">
+        <v>1907</v>
+      </c>
+      <c r="G15">
+        <v>1906</v>
+      </c>
+      <c r="H15">
+        <v>1968</v>
+      </c>
+      <c r="I15">
+        <v>1947</v>
+      </c>
+      <c r="J15">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>2286</v>
+      </c>
+      <c r="C16">
+        <v>2286</v>
+      </c>
+      <c r="D16">
+        <v>2286</v>
+      </c>
+      <c r="E16">
+        <v>1968</v>
+      </c>
+      <c r="F16">
+        <v>1968</v>
+      </c>
+      <c r="G16">
+        <v>1968</v>
+      </c>
+      <c r="H16">
+        <v>2025</v>
+      </c>
+      <c r="I16">
+        <v>1997</v>
+      </c>
+      <c r="J16">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>2374</v>
+      </c>
+      <c r="C17">
+        <v>2374</v>
+      </c>
+      <c r="D17">
+        <v>2374</v>
+      </c>
+      <c r="E17">
+        <v>2012</v>
+      </c>
+      <c r="F17">
+        <v>2010</v>
+      </c>
+      <c r="G17">
+        <v>2010</v>
+      </c>
+      <c r="H17">
+        <v>2072</v>
+      </c>
+      <c r="I17">
+        <v>2045</v>
+      </c>
+      <c r="J17">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18">
+        <v>2460</v>
+      </c>
+      <c r="C18">
+        <v>2460</v>
+      </c>
+      <c r="D18">
+        <v>2460</v>
+      </c>
+      <c r="E18">
+        <v>2058</v>
+      </c>
+      <c r="F18">
+        <v>2052</v>
+      </c>
+      <c r="G18">
+        <v>2059</v>
+      </c>
+      <c r="H18">
+        <v>2138</v>
+      </c>
+      <c r="I18">
+        <v>2097</v>
+      </c>
+      <c r="J18">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" t="s">
+        <v>31</v>
+      </c>
+      <c r="O22" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R22" t="s">
+        <v>36</v>
+      </c>
+      <c r="S22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23">
+        <v>2096</v>
+      </c>
+      <c r="C23">
+        <v>2146</v>
+      </c>
+      <c r="D23">
+        <v>2263</v>
+      </c>
+      <c r="E23">
+        <v>2286</v>
+      </c>
+      <c r="F23">
+        <v>2374</v>
+      </c>
+      <c r="G23">
+        <v>2460</v>
+      </c>
+      <c r="H23">
+        <v>1762</v>
+      </c>
+      <c r="I23">
+        <v>1810</v>
+      </c>
+      <c r="J23">
+        <v>1906</v>
+      </c>
+      <c r="K23">
+        <v>1968</v>
+      </c>
+      <c r="L23">
+        <v>2012</v>
+      </c>
+      <c r="M23">
+        <v>2058</v>
+      </c>
+      <c r="N23">
+        <v>1811</v>
+      </c>
+      <c r="O23">
+        <v>1858</v>
+      </c>
+      <c r="P23">
+        <v>1968</v>
+      </c>
+      <c r="Q23">
+        <v>2025</v>
+      </c>
+      <c r="R23">
+        <v>2072</v>
+      </c>
+      <c r="S23">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24">
+        <v>2096</v>
+      </c>
+      <c r="C24">
+        <v>2146</v>
+      </c>
+      <c r="D24">
+        <v>2263</v>
+      </c>
+      <c r="E24">
+        <v>2286</v>
+      </c>
+      <c r="F24">
+        <v>2374</v>
+      </c>
+      <c r="G24">
+        <v>2460</v>
+      </c>
+      <c r="H24">
+        <v>1758</v>
+      </c>
+      <c r="I24">
+        <v>1809</v>
+      </c>
+      <c r="J24">
+        <v>1907</v>
+      </c>
+      <c r="K24">
+        <v>1968</v>
+      </c>
+      <c r="L24">
+        <v>2010</v>
+      </c>
+      <c r="M24">
+        <v>2052</v>
+      </c>
+      <c r="N24">
+        <v>1784</v>
+      </c>
+      <c r="O24">
+        <v>1839</v>
+      </c>
+      <c r="P24">
+        <v>1947</v>
+      </c>
+      <c r="Q24">
+        <v>1997</v>
+      </c>
+      <c r="R24">
+        <v>2045</v>
+      </c>
+      <c r="S24">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>2096</v>
+      </c>
+      <c r="C25">
+        <v>2146</v>
+      </c>
+      <c r="D25">
+        <v>2263</v>
+      </c>
+      <c r="E25">
+        <v>2286</v>
+      </c>
+      <c r="F25">
+        <v>2374</v>
+      </c>
+      <c r="G25">
+        <v>2460</v>
+      </c>
+      <c r="H25">
+        <v>1761</v>
+      </c>
+      <c r="I25">
+        <v>1808</v>
+      </c>
+      <c r="J25">
+        <v>1906</v>
+      </c>
+      <c r="K25">
+        <v>1968</v>
+      </c>
+      <c r="L25">
+        <v>2010</v>
+      </c>
+      <c r="M25">
+        <v>2059</v>
+      </c>
+      <c r="N25">
+        <v>1771</v>
+      </c>
+      <c r="O25">
+        <v>1819</v>
+      </c>
+      <c r="P25">
+        <v>1923</v>
+      </c>
+      <c r="Q25">
+        <v>1987</v>
+      </c>
+      <c r="R25">
+        <v>2026</v>
+      </c>
+      <c r="S25">
+        <v>2076</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="N21:S21"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="E11:G11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>